<commit_message>
Updated self grading sheet.
</commit_message>
<xml_diff>
--- a/Super Castlevania 4/Vanhaverbeke_Brenainn_Super_Castlevania_IV.xlsx
+++ b/Super Castlevania 4/Vanhaverbeke_Brenainn_Super_Castlevania_IV.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">Game</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t xml:space="preserve">Load level from a file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External library</t>
   </si>
   <si>
     <t xml:space="preserve">Bone animation</t>
@@ -343,17 +346,17 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74"/>
   </cols>
   <sheetData>
@@ -373,7 +376,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -391,7 +394,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -400,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -409,7 +412,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -454,13 +457,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="74"/>
   </cols>
   <sheetData>
@@ -498,10 +501,13 @@
       <c r="B4" s="5" t="n">
         <v>1</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5" t="n">
         <v>0</v>
@@ -509,7 +515,7 @@
     </row>
     <row r="6" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>0</v>
@@ -517,7 +523,7 @@
     </row>
     <row r="7" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="5" t="n">
         <v>0</v>
@@ -525,7 +531,7 @@
     </row>
     <row r="8" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>0</v>
@@ -533,7 +539,7 @@
     </row>
     <row r="9" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0</v>
@@ -541,7 +547,7 @@
     </row>
     <row r="10" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>0</v>
@@ -549,7 +555,7 @@
     </row>
     <row r="11" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>0</v>
@@ -557,7 +563,7 @@
     </row>
     <row r="12" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5" t="n">
         <v>0</v>

</xml_diff>